<commit_message>
ml model and flask api initiated
</commit_message>
<xml_diff>
--- a/ai/datasets/final.xlsx
+++ b/ai/datasets/final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\Projects\Serenova\ai\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD1322B-66D7-4E0F-8127-BC4104C04582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F750B66-E197-4D6B-AB37-268D251D2FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FA46C6C7-2DD7-4CA4-97C9-37B09E91118D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{FA46C6C7-2DD7-4CA4-97C9-37B09E91118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,18 +50,9 @@
     <t>Light Intensity</t>
   </si>
   <si>
-    <t>Traffic density</t>
-  </si>
-  <si>
-    <t>Crowd density</t>
-  </si>
-  <si>
     <t>Crime Rate</t>
   </si>
   <si>
-    <t>Accidents</t>
-  </si>
-  <si>
     <t>Safety score</t>
   </si>
   <si>
@@ -270,6 +261,15 @@
   </si>
   <si>
     <t>Crime against women</t>
+  </si>
+  <si>
+    <t>Traffic Density</t>
+  </si>
+  <si>
+    <t>Crowd Density</t>
+  </si>
+  <si>
+    <t>Accident Rate</t>
   </si>
 </sst>
 </file>
@@ -305,10 +305,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +647,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,27 +666,27 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>20.931999999999999</v>
@@ -696,10 +697,28 @@
       <c r="D2" s="1">
         <v>0.81</v>
       </c>
+      <c r="E2">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="F2">
+        <v>43.01</v>
+      </c>
+      <c r="G2">
+        <v>69.91</v>
+      </c>
+      <c r="H2">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="I2">
+        <v>10.88</v>
+      </c>
+      <c r="J2" s="3">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>13.2172</v>
@@ -710,10 +729,28 @@
       <c r="D3" s="1">
         <v>0.95</v>
       </c>
+      <c r="E3">
+        <v>56.09</v>
+      </c>
+      <c r="F3">
+        <v>75.849999999999994</v>
+      </c>
+      <c r="G3">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="H3">
+        <v>34.979999999999997</v>
+      </c>
+      <c r="I3">
+        <v>41.01</v>
+      </c>
+      <c r="J3" s="3">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>16.5062</v>
@@ -724,10 +761,28 @@
       <c r="D4" s="2">
         <v>0.22</v>
       </c>
+      <c r="E4">
+        <v>90.79</v>
+      </c>
+      <c r="F4">
+        <v>27.9</v>
+      </c>
+      <c r="G4">
+        <v>61.23</v>
+      </c>
+      <c r="H4">
+        <v>24.65</v>
+      </c>
+      <c r="I4">
+        <v>27.39</v>
+      </c>
+      <c r="J4" s="3">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>17.686800000000002</v>
@@ -738,10 +793,28 @@
       <c r="D5" s="1">
         <v>0.95</v>
       </c>
+      <c r="E5">
+        <v>39.78</v>
+      </c>
+      <c r="F5">
+        <v>41.35</v>
+      </c>
+      <c r="G5">
+        <v>17.04</v>
+      </c>
+      <c r="H5">
+        <v>35.51</v>
+      </c>
+      <c r="I5">
+        <v>40.86</v>
+      </c>
+      <c r="J5" s="3">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>27.084399999999999</v>
@@ -752,10 +825,28 @@
       <c r="D6" s="2">
         <v>0.38500000000000001</v>
       </c>
+      <c r="E6">
+        <v>36.31</v>
+      </c>
+      <c r="F6">
+        <v>46.77</v>
+      </c>
+      <c r="G6">
+        <v>85.79</v>
+      </c>
+      <c r="H6">
+        <v>77.959999999999994</v>
+      </c>
+      <c r="I6">
+        <v>43.39</v>
+      </c>
+      <c r="J6" s="3">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>23.1433</v>
@@ -766,10 +857,28 @@
       <c r="D7" s="2">
         <v>0.20660000000000001</v>
       </c>
+      <c r="E7">
+        <v>91.12</v>
+      </c>
+      <c r="F7">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="G7">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="H7">
+        <v>60.99</v>
+      </c>
+      <c r="I7">
+        <v>43.41</v>
+      </c>
+      <c r="J7" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>26.1158</v>
@@ -780,10 +889,28 @@
       <c r="D8" s="1">
         <v>0.53</v>
       </c>
+      <c r="E8">
+        <v>45.27</v>
+      </c>
+      <c r="F8">
+        <v>38.090000000000003</v>
+      </c>
+      <c r="G8">
+        <v>82.75</v>
+      </c>
+      <c r="H8">
+        <v>14.85</v>
+      </c>
+      <c r="I8">
+        <v>16.95</v>
+      </c>
+      <c r="J8" s="3">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>26.643799999999999</v>
@@ -794,10 +921,28 @@
       <c r="D9" s="1">
         <v>0.2</v>
       </c>
+      <c r="E9">
+        <v>49.8</v>
+      </c>
+      <c r="F9">
+        <v>92.69</v>
+      </c>
+      <c r="G9">
+        <v>70.5</v>
+      </c>
+      <c r="H9">
+        <v>22.01</v>
+      </c>
+      <c r="I9">
+        <v>23.25</v>
+      </c>
+      <c r="J9" s="3">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>25.594100000000001</v>
@@ -808,10 +953,28 @@
       <c r="D10" s="1">
         <v>0.72</v>
       </c>
+      <c r="E10">
+        <v>34.32</v>
+      </c>
+      <c r="F10">
+        <v>58.49</v>
+      </c>
+      <c r="G10">
+        <v>11.17</v>
+      </c>
+      <c r="H10">
+        <v>100.91</v>
+      </c>
+      <c r="I10">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="J10" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>30.7333</v>
@@ -822,10 +985,28 @@
       <c r="D11" s="1">
         <v>0.53</v>
       </c>
+      <c r="E11">
+        <v>25.89</v>
+      </c>
+      <c r="F11">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="G11">
+        <v>47.81</v>
+      </c>
+      <c r="H11">
+        <v>80.430000000000007</v>
+      </c>
+      <c r="I11">
+        <v>66.27</v>
+      </c>
+      <c r="J11" s="3">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>21.2514</v>
@@ -836,10 +1017,28 @@
       <c r="D12" s="1">
         <v>0.15</v>
       </c>
+      <c r="E12">
+        <v>21.59</v>
+      </c>
+      <c r="F12">
+        <v>87.25</v>
+      </c>
+      <c r="G12">
+        <v>31.85</v>
+      </c>
+      <c r="H12">
+        <v>42.97</v>
+      </c>
+      <c r="I12">
+        <v>88.58</v>
+      </c>
+      <c r="J12" s="3">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>28.7041</v>
@@ -850,10 +1049,28 @@
       <c r="D13" s="1">
         <v>0.98</v>
       </c>
+      <c r="E13">
+        <v>18.59</v>
+      </c>
+      <c r="F13">
+        <v>95.88</v>
+      </c>
+      <c r="G13">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H13">
+        <v>57.31</v>
+      </c>
+      <c r="I13">
+        <v>13.19</v>
+      </c>
+      <c r="J13" s="3">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>28.613900000000001</v>
@@ -864,10 +1081,28 @@
       <c r="D14" s="1">
         <v>0.99</v>
       </c>
+      <c r="E14">
+        <v>55.5</v>
+      </c>
+      <c r="F14">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="G14">
+        <v>63.43</v>
+      </c>
+      <c r="H14">
+        <v>82.94</v>
+      </c>
+      <c r="I14">
+        <v>99.02</v>
+      </c>
+      <c r="J14" s="3">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>15.299300000000001</v>
@@ -878,10 +1113,28 @@
       <c r="D15" s="1">
         <v>0.65</v>
       </c>
+      <c r="E15">
+        <v>51.44</v>
+      </c>
+      <c r="F15">
+        <v>62.55</v>
+      </c>
+      <c r="G15">
+        <v>85.93</v>
+      </c>
+      <c r="H15">
+        <v>80.34</v>
+      </c>
+      <c r="I15">
+        <v>50.18</v>
+      </c>
+      <c r="J15" s="3">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>23.022500000000001</v>
@@ -892,10 +1145,28 @@
       <c r="D16" s="2">
         <v>0.98599999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>53.14</v>
+      </c>
+      <c r="F16">
+        <v>50.42</v>
+      </c>
+      <c r="G16">
+        <v>31.98</v>
+      </c>
+      <c r="H16">
+        <v>49.99</v>
+      </c>
+      <c r="I16">
+        <v>88.19</v>
+      </c>
+      <c r="J16" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>28.5823</v>
@@ -906,10 +1177,28 @@
       <c r="D17" s="1">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>38.28</v>
+      </c>
+      <c r="F17">
+        <v>60.48</v>
+      </c>
+      <c r="G17">
+        <v>18.11</v>
+      </c>
+      <c r="H17">
+        <v>25.29</v>
+      </c>
+      <c r="I17">
+        <v>26.36</v>
+      </c>
+      <c r="J17" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>23.215599999999998</v>
@@ -920,10 +1209,28 @@
       <c r="D18" s="1">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>74.67</v>
+      </c>
+      <c r="F18">
+        <v>84.05</v>
+      </c>
+      <c r="G18">
+        <v>57.72</v>
+      </c>
+      <c r="H18">
+        <v>86.89</v>
+      </c>
+      <c r="I18">
+        <v>79.09</v>
+      </c>
+      <c r="J18" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>22.470700000000001</v>
@@ -934,10 +1241,28 @@
       <c r="D19" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>46.03</v>
+      </c>
+      <c r="F19">
+        <v>85.58</v>
+      </c>
+      <c r="G19">
+        <v>15.42</v>
+      </c>
+      <c r="H19">
+        <v>51.14</v>
+      </c>
+      <c r="I19">
+        <v>22.74</v>
+      </c>
+      <c r="J19" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>21.522200000000002</v>
@@ -948,10 +1273,28 @@
       <c r="D20" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>29.52</v>
+      </c>
+      <c r="F20">
+        <v>80.03</v>
+      </c>
+      <c r="G20">
+        <v>28.88</v>
+      </c>
+      <c r="H20">
+        <v>77.98</v>
+      </c>
+      <c r="I20">
+        <v>42.69</v>
+      </c>
+      <c r="J20" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>22.303899999999999</v>
@@ -962,10 +1305,28 @@
       <c r="D21" s="1">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>76.56</v>
+      </c>
+      <c r="F21">
+        <v>24.03</v>
+      </c>
+      <c r="G21">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="H21">
+        <v>100.9</v>
+      </c>
+      <c r="I21">
+        <v>83.25</v>
+      </c>
+      <c r="J21" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>21.170200000000001</v>
@@ -976,10 +1337,28 @@
       <c r="D22" s="1">
         <v>0.98699999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>14.18</v>
+      </c>
+      <c r="F22">
+        <v>54.4</v>
+      </c>
+      <c r="G22">
+        <v>56.96</v>
+      </c>
+      <c r="H22">
+        <v>83.77</v>
+      </c>
+      <c r="I22">
+        <v>51</v>
+      </c>
+      <c r="J22" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>20.5992</v>
@@ -990,10 +1369,28 @@
       <c r="D23" s="1">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>93.36</v>
+      </c>
+      <c r="G23">
+        <v>59.82</v>
+      </c>
+      <c r="H23">
+        <v>85.62</v>
+      </c>
+      <c r="I23">
+        <v>64.34</v>
+      </c>
+      <c r="J23" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>28.408899999999999</v>
@@ -1004,10 +1401,28 @@
       <c r="D24" s="1">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>39.86</v>
+      </c>
+      <c r="F24">
+        <v>40.96</v>
+      </c>
+      <c r="G24">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="H24">
+        <v>46.71</v>
+      </c>
+      <c r="I24">
+        <v>39.54</v>
+      </c>
+      <c r="J24" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>30.9331</v>
@@ -1018,10 +1433,28 @@
       <c r="D25" s="1">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>81.069999999999993</v>
+      </c>
+      <c r="F25">
+        <v>94.98</v>
+      </c>
+      <c r="G25">
+        <v>36.78</v>
+      </c>
+      <c r="H25">
+        <v>40.26</v>
+      </c>
+      <c r="I25">
+        <v>92.98</v>
+      </c>
+      <c r="J25" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>28.459499999999998</v>
@@ -1032,10 +1465,28 @@
       <c r="D26" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>66.790000000000006</v>
+      </c>
+      <c r="F26">
+        <v>55.86</v>
+      </c>
+      <c r="G26">
+        <v>15.13</v>
+      </c>
+      <c r="H26">
+        <v>63.63</v>
+      </c>
+      <c r="I26">
+        <v>64.59</v>
+      </c>
+      <c r="J26" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>29.325500000000002</v>
@@ -1046,10 +1497,28 @@
       <c r="D27" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>98.02</v>
+      </c>
+      <c r="F27">
+        <v>91.42</v>
+      </c>
+      <c r="G27">
+        <v>71.7</v>
+      </c>
+      <c r="H27">
+        <v>65.39</v>
+      </c>
+      <c r="I27">
+        <v>98.47</v>
+      </c>
+      <c r="J27" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>29.685700000000001</v>
@@ -1060,10 +1529,28 @@
       <c r="D28" s="1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>43.34</v>
+      </c>
+      <c r="F28">
+        <v>71.73</v>
+      </c>
+      <c r="G28">
+        <v>62.07</v>
+      </c>
+      <c r="H28">
+        <v>36.39</v>
+      </c>
+      <c r="I28">
+        <v>77.64</v>
+      </c>
+      <c r="J28" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>29.9695</v>
@@ -1074,10 +1561,28 @@
       <c r="D29" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>90</v>
+      </c>
+      <c r="F29">
+        <v>86.38</v>
+      </c>
+      <c r="G29">
+        <v>63.62</v>
+      </c>
+      <c r="H29">
+        <v>15.21</v>
+      </c>
+      <c r="I29">
+        <v>89.45</v>
+      </c>
+      <c r="J29" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>28.192</v>
@@ -1088,10 +1593,28 @@
       <c r="D30" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>87.76</v>
+      </c>
+      <c r="F30">
+        <v>66.22</v>
+      </c>
+      <c r="G30">
+        <v>11.48</v>
+      </c>
+      <c r="H30">
+        <v>58.54</v>
+      </c>
+      <c r="I30">
+        <v>48.27</v>
+      </c>
+      <c r="J30" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>28.895499999999998</v>
@@ -1102,10 +1625,28 @@
       <c r="D31" s="1">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>85.02</v>
+      </c>
+      <c r="F31">
+        <v>12.82</v>
+      </c>
+      <c r="G31">
+        <v>48.71</v>
+      </c>
+      <c r="H31">
+        <v>47.83</v>
+      </c>
+      <c r="I31">
+        <v>26.09</v>
+      </c>
+      <c r="J31" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>29.5321</v>
@@ -1116,10 +1657,28 @@
       <c r="D32" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>25.68</v>
+      </c>
+      <c r="F32">
+        <v>31.7</v>
+      </c>
+      <c r="G32">
+        <v>62.25</v>
+      </c>
+      <c r="H32">
+        <v>24.79</v>
+      </c>
+      <c r="I32">
+        <v>39.83</v>
+      </c>
+      <c r="J32" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>28.993099999999998</v>
@@ -1130,10 +1689,28 @@
       <c r="D33" s="1">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>58.51</v>
+      </c>
+      <c r="F33">
+        <v>97.12</v>
+      </c>
+      <c r="G33">
+        <v>93.41</v>
+      </c>
+      <c r="H33">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="I33">
+        <v>26.28</v>
+      </c>
+      <c r="J33" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>32.726599999999998</v>
@@ -1144,10 +1721,28 @@
       <c r="D34" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>63.03</v>
+      </c>
+      <c r="F34">
+        <v>77.510000000000005</v>
+      </c>
+      <c r="G34">
+        <v>82.39</v>
+      </c>
+      <c r="H34">
+        <v>82.52</v>
+      </c>
+      <c r="I34">
+        <v>28.02</v>
+      </c>
+      <c r="J34" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>23.691299999999998</v>
@@ -1158,10 +1753,28 @@
       <c r="D35" s="1">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>24.24</v>
+      </c>
+      <c r="F35">
+        <v>50.13</v>
+      </c>
+      <c r="G35">
+        <v>94.87</v>
+      </c>
+      <c r="H35">
+        <v>55.15</v>
+      </c>
+      <c r="I35">
+        <v>38.880000000000003</v>
+      </c>
+      <c r="J35" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>15.317299999999999</v>
@@ -1172,10 +1785,28 @@
       <c r="D36" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>63.31</v>
+      </c>
+      <c r="F36">
+        <v>13.18</v>
+      </c>
+      <c r="G36">
+        <v>42.57</v>
+      </c>
+      <c r="H36">
+        <v>26.68</v>
+      </c>
+      <c r="I36">
+        <v>36.409999999999997</v>
+      </c>
+      <c r="J36" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>10.1632</v>
@@ -1186,10 +1817,28 @@
       <c r="D37" s="1">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>25.2</v>
+      </c>
+      <c r="F37">
+        <v>85.15</v>
+      </c>
+      <c r="G37">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="H37">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="I37">
+        <v>85.79</v>
+      </c>
+      <c r="J37" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>22.973400000000002</v>
@@ -1200,10 +1849,28 @@
       <c r="D38" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>32.42</v>
+      </c>
+      <c r="F38">
+        <v>28.91</v>
+      </c>
+      <c r="G38">
+        <v>80.45</v>
+      </c>
+      <c r="H38">
+        <v>100.79</v>
+      </c>
+      <c r="I38">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="J38" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>19.7515</v>
@@ -1214,10 +1881,28 @@
       <c r="D39" s="1">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>79.67</v>
+      </c>
+      <c r="F39">
+        <v>20.65</v>
+      </c>
+      <c r="G39">
+        <v>71.37</v>
+      </c>
+      <c r="H39">
+        <v>69.8</v>
+      </c>
+      <c r="I39">
+        <v>32.46</v>
+      </c>
+      <c r="J39" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>19.076000000000001</v>
@@ -1228,10 +1913,28 @@
       <c r="D40" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>29.41</v>
+      </c>
+      <c r="F40">
+        <v>79.239999999999995</v>
+      </c>
+      <c r="G40">
+        <v>14.47</v>
+      </c>
+      <c r="H40">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="I40">
+        <v>100.84</v>
+      </c>
+      <c r="J40" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>18.520399999999999</v>
@@ -1242,10 +1945,28 @@
       <c r="D41" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>79.27</v>
+      </c>
+      <c r="F41">
+        <v>96.07</v>
+      </c>
+      <c r="G41">
+        <v>81.62</v>
+      </c>
+      <c r="H41">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="I41">
+        <v>17.079999999999998</v>
+      </c>
+      <c r="J41" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>20.2376</v>
@@ -1256,10 +1977,28 @@
       <c r="D42" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>12.7</v>
+      </c>
+      <c r="F42">
+        <v>40.43</v>
+      </c>
+      <c r="G42">
+        <v>69.38</v>
+      </c>
+      <c r="H42">
+        <v>30.86</v>
+      </c>
+      <c r="I42">
+        <v>70.78</v>
+      </c>
+      <c r="J42" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>11.941599999999999</v>
@@ -1270,10 +2009,28 @@
       <c r="D43" s="1">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>82.22</v>
+      </c>
+      <c r="F43">
+        <v>32.39</v>
+      </c>
+      <c r="G43">
+        <v>32.619999999999997</v>
+      </c>
+      <c r="H43">
+        <v>12.44</v>
+      </c>
+      <c r="I43">
+        <v>87.04</v>
+      </c>
+      <c r="J43" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>20.295999999999999</v>
@@ -1284,10 +2041,28 @@
       <c r="D44" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>91.3</v>
+      </c>
+      <c r="F44">
+        <v>14.12</v>
+      </c>
+      <c r="G44">
+        <v>20.6</v>
+      </c>
+      <c r="H44">
+        <v>90.1</v>
+      </c>
+      <c r="I44">
+        <v>78.19</v>
+      </c>
+      <c r="J44" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>31.147099999999998</v>
@@ -1298,10 +2073,28 @@
       <c r="D45" s="1">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>24.29</v>
+      </c>
+      <c r="F45">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="G45">
+        <v>87.09</v>
+      </c>
+      <c r="H45">
+        <v>99.17</v>
+      </c>
+      <c r="I45">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="J45" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>31.634</v>
@@ -1312,10 +2105,28 @@
       <c r="D46" s="1">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>97.48</v>
+      </c>
+      <c r="F46">
+        <v>92.08</v>
+      </c>
+      <c r="G46">
+        <v>10.92</v>
+      </c>
+      <c r="H46">
+        <v>22.68</v>
+      </c>
+      <c r="I46">
+        <v>99.14</v>
+      </c>
+      <c r="J46" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <v>31.326000000000001</v>
@@ -1326,10 +2137,28 @@
       <c r="D47" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>59.8</v>
+      </c>
+      <c r="F47">
+        <v>55.25</v>
+      </c>
+      <c r="G47">
+        <v>86.8</v>
+      </c>
+      <c r="H47">
+        <v>60.5</v>
+      </c>
+      <c r="I47">
+        <v>11.61</v>
+      </c>
+      <c r="J47" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>30.901</v>
@@ -1340,10 +2169,28 @@
       <c r="D48" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>16.46</v>
+      </c>
+      <c r="F48">
+        <v>89.12</v>
+      </c>
+      <c r="G48">
+        <v>61.8</v>
+      </c>
+      <c r="H48">
+        <v>95.17</v>
+      </c>
+      <c r="I48">
+        <v>38.19</v>
+      </c>
+      <c r="J48" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>31.372299999999999</v>
@@ -1354,10 +2201,28 @@
       <c r="D49" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>95.88</v>
+      </c>
+      <c r="F49">
+        <v>29.89</v>
+      </c>
+      <c r="G49">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="H49">
+        <v>28.12</v>
+      </c>
+      <c r="I49">
+        <v>58.88</v>
+      </c>
+      <c r="J49" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>30.373000000000001</v>
@@ -1368,10 +2233,28 @@
       <c r="D50" s="1">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="F50">
+        <v>42.42</v>
+      </c>
+      <c r="G50">
+        <v>59.84</v>
+      </c>
+      <c r="H50">
+        <v>95.76</v>
+      </c>
+      <c r="I50">
+        <v>70.709999999999994</v>
+      </c>
+      <c r="J50" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>30.2438</v>
@@ -1382,10 +2265,28 @@
       <c r="D51" s="1">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>59.22</v>
+      </c>
+      <c r="F51">
+        <v>35.1</v>
+      </c>
+      <c r="G51">
+        <v>31.88</v>
+      </c>
+      <c r="H51">
+        <v>19.09</v>
+      </c>
+      <c r="I51">
+        <v>95.51</v>
+      </c>
+      <c r="J51" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B52">
         <v>30.3398</v>
@@ -1396,10 +2297,28 @@
       <c r="D52" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>32.64</v>
+      </c>
+      <c r="F52">
+        <v>61.51</v>
+      </c>
+      <c r="G52">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H52">
+        <v>68.83</v>
+      </c>
+      <c r="I52">
+        <v>99.46</v>
+      </c>
+      <c r="J52" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B53">
         <v>27.023800000000001</v>
@@ -1410,10 +2329,28 @@
       <c r="D53" s="1">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>98.85</v>
+      </c>
+      <c r="F53">
+        <v>63.12</v>
+      </c>
+      <c r="G53">
+        <v>58.75</v>
+      </c>
+      <c r="H53">
+        <v>99.65</v>
+      </c>
+      <c r="I53">
+        <v>86.42</v>
+      </c>
+      <c r="J53" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54">
         <v>24.5854</v>
@@ -1424,10 +2361,28 @@
       <c r="D54" s="1">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>85</v>
+      </c>
+      <c r="F54">
+        <v>30.82</v>
+      </c>
+      <c r="G54">
+        <v>14.15</v>
+      </c>
+      <c r="H54">
+        <v>21.75</v>
+      </c>
+      <c r="I54">
+        <v>13.41</v>
+      </c>
+      <c r="J54" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>11.1271</v>
@@ -1438,10 +2393,28 @@
       <c r="D55" s="1">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="F55">
+        <v>83.2</v>
+      </c>
+      <c r="G55">
+        <v>33.53</v>
+      </c>
+      <c r="H55">
+        <v>36.770000000000003</v>
+      </c>
+      <c r="I55">
+        <v>70.180000000000007</v>
+      </c>
+      <c r="J55" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>18.112400000000001</v>
@@ -1452,10 +2425,28 @@
       <c r="D56" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>56.65</v>
+      </c>
+      <c r="F56">
+        <v>92.42</v>
+      </c>
+      <c r="G56">
+        <v>41.85</v>
+      </c>
+      <c r="H56">
+        <v>33</v>
+      </c>
+      <c r="I56">
+        <v>93.63</v>
+      </c>
+      <c r="J56" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>27.570599999999999</v>
@@ -1466,10 +2457,28 @@
       <c r="D57" s="1">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>18.86</v>
+      </c>
+      <c r="F57">
+        <v>24.56</v>
+      </c>
+      <c r="G57">
+        <v>55.63</v>
+      </c>
+      <c r="H57">
+        <v>56.16</v>
+      </c>
+      <c r="I57">
+        <v>85.99</v>
+      </c>
+      <c r="J57" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>26.792200000000001</v>
@@ -1480,10 +2489,28 @@
       <c r="D58" s="1">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>15.94</v>
+      </c>
+      <c r="F58">
+        <v>87.1</v>
+      </c>
+      <c r="G58">
+        <v>10.15</v>
+      </c>
+      <c r="H58">
+        <v>31.74</v>
+      </c>
+      <c r="I58">
+        <v>65.41</v>
+      </c>
+      <c r="J58" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B59">
         <v>27.1767</v>
@@ -1494,10 +2521,28 @@
       <c r="D59" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>45.97</v>
+      </c>
+      <c r="F59">
+        <v>72.45</v>
+      </c>
+      <c r="G59">
+        <v>52.74</v>
+      </c>
+      <c r="H59">
+        <v>53.24</v>
+      </c>
+      <c r="I59">
+        <v>45.53</v>
+      </c>
+      <c r="J59" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>25.448799999999999</v>
@@ -1508,10 +2553,28 @@
       <c r="D60" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>45.04</v>
+      </c>
+      <c r="F60">
+        <v>78.5</v>
+      </c>
+      <c r="G60">
+        <v>64.349999999999994</v>
+      </c>
+      <c r="H60">
+        <v>84.7</v>
+      </c>
+      <c r="I60">
+        <v>38.06</v>
+      </c>
+      <c r="J60" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>26.846699999999998</v>
@@ -1522,10 +2585,28 @@
       <c r="D61" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>66.39</v>
+      </c>
+      <c r="F61">
+        <v>40.950000000000003</v>
+      </c>
+      <c r="G61">
+        <v>56.05</v>
+      </c>
+      <c r="H61">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="I61">
+        <v>61.47</v>
+      </c>
+      <c r="J61" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>27.4924</v>
@@ -1536,10 +2617,28 @@
       <c r="D62" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>45.73</v>
+      </c>
+      <c r="F62">
+        <v>10.47</v>
+      </c>
+      <c r="G62">
+        <v>92.98</v>
+      </c>
+      <c r="H62">
+        <v>72.36</v>
+      </c>
+      <c r="I62">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="J62" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>28.984500000000001</v>
@@ -1550,10 +2649,28 @@
       <c r="D63" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>35.92</v>
+      </c>
+      <c r="F63">
+        <v>69.48</v>
+      </c>
+      <c r="G63">
+        <v>45.49</v>
+      </c>
+      <c r="H63">
+        <v>77.290000000000006</v>
+      </c>
+      <c r="I63">
+        <v>50.44</v>
+      </c>
+      <c r="J63" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B64">
         <v>25.468299999999999</v>
@@ -1564,10 +2681,28 @@
       <c r="D64" s="1">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>49.45</v>
+      </c>
+      <c r="F64">
+        <v>74.44</v>
+      </c>
+      <c r="G64">
+        <v>18.47</v>
+      </c>
+      <c r="H64">
+        <v>82.36</v>
+      </c>
+      <c r="I64">
+        <v>46.99</v>
+      </c>
+      <c r="J64" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>25.317599999999999</v>
@@ -1578,10 +2713,28 @@
       <c r="D65" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F65">
+        <v>25.13</v>
+      </c>
+      <c r="G65">
+        <v>44.54</v>
+      </c>
+      <c r="H65">
+        <v>80.91</v>
+      </c>
+      <c r="I65">
+        <v>81.92</v>
+      </c>
+      <c r="J65" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>30.066800000000001</v>
@@ -1592,10 +2745,28 @@
       <c r="D66" s="1">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <v>44.26</v>
+      </c>
+      <c r="F66">
+        <v>61.21</v>
+      </c>
+      <c r="G66">
+        <v>52.83</v>
+      </c>
+      <c r="H66">
+        <v>62.27</v>
+      </c>
+      <c r="I66">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="J66" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>30.316500000000001</v>
@@ -1606,10 +2777,28 @@
       <c r="D67" s="1">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>25.41</v>
+      </c>
+      <c r="F67">
+        <v>93.24</v>
+      </c>
+      <c r="G67">
+        <v>24.89</v>
+      </c>
+      <c r="H67">
+        <v>75.98</v>
+      </c>
+      <c r="I67">
+        <v>16.18</v>
+      </c>
+      <c r="J67" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>29.945699999999999</v>
@@ -1620,10 +2809,28 @@
       <c r="D68" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>63.3</v>
+      </c>
+      <c r="F68">
+        <v>32.6</v>
+      </c>
+      <c r="G68">
+        <v>29.88</v>
+      </c>
+      <c r="H68">
+        <v>55.98</v>
+      </c>
+      <c r="I68">
+        <v>49.38</v>
+      </c>
+      <c r="J68" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B69">
         <v>22.986799999999999</v>
@@ -1633,6 +2840,24 @@
       </c>
       <c r="D69" s="1">
         <v>0.81</v>
+      </c>
+      <c r="E69">
+        <v>67.8</v>
+      </c>
+      <c r="F69">
+        <v>25.98</v>
+      </c>
+      <c r="G69">
+        <v>63.36</v>
+      </c>
+      <c r="H69">
+        <v>86.88</v>
+      </c>
+      <c r="I69">
+        <v>59.26</v>
+      </c>
+      <c r="J69" s="3">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enhance route scoring functionality and data handling
- Updated dataset.csv to include new routes with relevant metrics.
- Modified RouteScorerForm component to submit route data to the server.
- Implemented addRoute function in user.controller.js to handle incoming route submissions and append them to dataset.csv.
- Added necessary CSV parsing and stringifying dependencies to package.json and package-lock.json.
- Updated routes.route.js to include a new endpoint for adding routes.
- Adjusted final.xlsx to reflect changes in the dataset.
</commit_message>
<xml_diff>
--- a/ai/datasets/final.xlsx
+++ b/ai/datasets/final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\Projects\Serenova\ai\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F750B66-E197-4D6B-AB37-268D251D2FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5488BA9A-9B8F-49C9-BA4E-DFB9896141FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{FA46C6C7-2DD7-4CA4-97C9-37B09E91118D}"/>
+    <workbookView xWindow="5760" yWindow="144" windowWidth="17280" windowHeight="9420" xr2:uid="{FA46C6C7-2DD7-4CA4-97C9-37B09E91118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>City</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Ahmedabad</t>
-  </si>
-  <si>
-    <t>Crime against women</t>
   </si>
   <si>
     <t>Traffic Density</t>
@@ -644,15 +641,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9009F197-4FC0-4A78-90EF-3BE4A8C26053}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,25 +663,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -709,14 +703,11 @@
       <c r="H2">
         <v>65.209999999999994</v>
       </c>
-      <c r="I2">
-        <v>10.88</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="I2" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -741,14 +732,11 @@
       <c r="H3">
         <v>34.979999999999997</v>
       </c>
-      <c r="I3">
-        <v>41.01</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="I3" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -773,14 +761,11 @@
       <c r="H4">
         <v>24.65</v>
       </c>
-      <c r="I4">
-        <v>27.39</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="I4" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -805,14 +790,11 @@
       <c r="H5">
         <v>35.51</v>
       </c>
-      <c r="I5">
-        <v>40.86</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="I5" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -837,14 +819,11 @@
       <c r="H6">
         <v>77.959999999999994</v>
       </c>
-      <c r="I6">
-        <v>43.39</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="I6" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -869,14 +848,11 @@
       <c r="H7">
         <v>60.99</v>
       </c>
-      <c r="I7">
-        <v>43.41</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="I7" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -901,14 +877,11 @@
       <c r="H8">
         <v>14.85</v>
       </c>
-      <c r="I8">
-        <v>16.95</v>
-      </c>
-      <c r="J8" s="3">
+      <c r="I8" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -933,14 +906,11 @@
       <c r="H9">
         <v>22.01</v>
       </c>
-      <c r="I9">
-        <v>23.25</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="I9" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -965,14 +935,11 @@
       <c r="H10">
         <v>100.91</v>
       </c>
-      <c r="I10">
-        <v>36.049999999999997</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="I10" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -997,14 +964,11 @@
       <c r="H11">
         <v>80.430000000000007</v>
       </c>
-      <c r="I11">
-        <v>66.27</v>
-      </c>
-      <c r="J11" s="3">
+      <c r="I11" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1029,14 +993,11 @@
       <c r="H12">
         <v>42.97</v>
       </c>
-      <c r="I12">
-        <v>88.58</v>
-      </c>
-      <c r="J12" s="3">
+      <c r="I12" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1061,14 +1022,11 @@
       <c r="H13">
         <v>57.31</v>
       </c>
-      <c r="I13">
-        <v>13.19</v>
-      </c>
-      <c r="J13" s="3">
+      <c r="I13" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1093,14 +1051,11 @@
       <c r="H14">
         <v>82.94</v>
       </c>
-      <c r="I14">
-        <v>99.02</v>
-      </c>
-      <c r="J14" s="3">
+      <c r="I14" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1125,14 +1080,11 @@
       <c r="H15">
         <v>80.34</v>
       </c>
-      <c r="I15">
-        <v>50.18</v>
-      </c>
-      <c r="J15" s="3">
+      <c r="I15" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1157,14 +1109,11 @@
       <c r="H16">
         <v>49.99</v>
       </c>
-      <c r="I16">
-        <v>88.19</v>
-      </c>
-      <c r="J16" s="3">
+      <c r="I16" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1189,14 +1138,11 @@
       <c r="H17">
         <v>25.29</v>
       </c>
-      <c r="I17">
-        <v>26.36</v>
-      </c>
-      <c r="J17" s="3">
+      <c r="I17" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1221,14 +1167,11 @@
       <c r="H18">
         <v>86.89</v>
       </c>
-      <c r="I18">
-        <v>79.09</v>
-      </c>
-      <c r="J18" s="3">
+      <c r="I18" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1253,14 +1196,11 @@
       <c r="H19">
         <v>51.14</v>
       </c>
-      <c r="I19">
-        <v>22.74</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="I19" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1285,14 +1225,11 @@
       <c r="H20">
         <v>77.98</v>
       </c>
-      <c r="I20">
-        <v>42.69</v>
-      </c>
-      <c r="J20" s="3">
+      <c r="I20" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1317,14 +1254,11 @@
       <c r="H21">
         <v>100.9</v>
       </c>
-      <c r="I21">
-        <v>83.25</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="I21" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1349,14 +1283,11 @@
       <c r="H22">
         <v>83.77</v>
       </c>
-      <c r="I22">
-        <v>51</v>
-      </c>
-      <c r="J22" s="3">
+      <c r="I22" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1381,14 +1312,11 @@
       <c r="H23">
         <v>85.62</v>
       </c>
-      <c r="I23">
-        <v>64.34</v>
-      </c>
-      <c r="J23" s="3">
+      <c r="I23" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1413,14 +1341,11 @@
       <c r="H24">
         <v>46.71</v>
       </c>
-      <c r="I24">
-        <v>39.54</v>
-      </c>
-      <c r="J24" s="3">
+      <c r="I24" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1445,14 +1370,11 @@
       <c r="H25">
         <v>40.26</v>
       </c>
-      <c r="I25">
-        <v>92.98</v>
-      </c>
-      <c r="J25" s="3">
+      <c r="I25" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1477,14 +1399,11 @@
       <c r="H26">
         <v>63.63</v>
       </c>
-      <c r="I26">
-        <v>64.59</v>
-      </c>
-      <c r="J26" s="3">
+      <c r="I26" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1509,14 +1428,11 @@
       <c r="H27">
         <v>65.39</v>
       </c>
-      <c r="I27">
-        <v>98.47</v>
-      </c>
-      <c r="J27" s="3">
+      <c r="I27" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1541,14 +1457,11 @@
       <c r="H28">
         <v>36.39</v>
       </c>
-      <c r="I28">
-        <v>77.64</v>
-      </c>
-      <c r="J28" s="3">
+      <c r="I28" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1573,14 +1486,11 @@
       <c r="H29">
         <v>15.21</v>
       </c>
-      <c r="I29">
-        <v>89.45</v>
-      </c>
-      <c r="J29" s="3">
+      <c r="I29" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1605,14 +1515,11 @@
       <c r="H30">
         <v>58.54</v>
       </c>
-      <c r="I30">
-        <v>48.27</v>
-      </c>
-      <c r="J30" s="3">
+      <c r="I30" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1637,14 +1544,11 @@
       <c r="H31">
         <v>47.83</v>
       </c>
-      <c r="I31">
-        <v>26.09</v>
-      </c>
-      <c r="J31" s="3">
+      <c r="I31" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1669,14 +1573,11 @@
       <c r="H32">
         <v>24.79</v>
       </c>
-      <c r="I32">
-        <v>39.83</v>
-      </c>
-      <c r="J32" s="3">
+      <c r="I32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1701,14 +1602,11 @@
       <c r="H33">
         <v>16.149999999999999</v>
       </c>
-      <c r="I33">
-        <v>26.28</v>
-      </c>
-      <c r="J33" s="3">
+      <c r="I33" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1733,14 +1631,11 @@
       <c r="H34">
         <v>82.52</v>
       </c>
-      <c r="I34">
-        <v>28.02</v>
-      </c>
-      <c r="J34" s="3">
+      <c r="I34" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1765,14 +1660,11 @@
       <c r="H35">
         <v>55.15</v>
       </c>
-      <c r="I35">
-        <v>38.880000000000003</v>
-      </c>
-      <c r="J35" s="3">
+      <c r="I35" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1797,14 +1689,11 @@
       <c r="H36">
         <v>26.68</v>
       </c>
-      <c r="I36">
-        <v>36.409999999999997</v>
-      </c>
-      <c r="J36" s="3">
+      <c r="I36" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1829,14 +1718,11 @@
       <c r="H37">
         <v>79.010000000000005</v>
       </c>
-      <c r="I37">
-        <v>85.79</v>
-      </c>
-      <c r="J37" s="3">
+      <c r="I37" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1861,14 +1747,11 @@
       <c r="H38">
         <v>100.79</v>
       </c>
-      <c r="I38">
-        <v>19.170000000000002</v>
-      </c>
-      <c r="J38" s="3">
+      <c r="I38" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1893,14 +1776,11 @@
       <c r="H39">
         <v>69.8</v>
       </c>
-      <c r="I39">
-        <v>32.46</v>
-      </c>
-      <c r="J39" s="3">
+      <c r="I39" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1925,14 +1805,11 @@
       <c r="H40">
         <v>65.900000000000006</v>
       </c>
-      <c r="I40">
-        <v>100.84</v>
-      </c>
-      <c r="J40" s="3">
+      <c r="I40" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1957,14 +1834,11 @@
       <c r="H41">
         <v>38.299999999999997</v>
       </c>
-      <c r="I41">
-        <v>17.079999999999998</v>
-      </c>
-      <c r="J41" s="3">
+      <c r="I41" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1989,14 +1863,11 @@
       <c r="H42">
         <v>30.86</v>
       </c>
-      <c r="I42">
-        <v>70.78</v>
-      </c>
-      <c r="J42" s="3">
+      <c r="I42" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -2021,14 +1892,11 @@
       <c r="H43">
         <v>12.44</v>
       </c>
-      <c r="I43">
-        <v>87.04</v>
-      </c>
-      <c r="J43" s="3">
+      <c r="I43" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2053,14 +1921,11 @@
       <c r="H44">
         <v>90.1</v>
       </c>
-      <c r="I44">
-        <v>78.19</v>
-      </c>
-      <c r="J44" s="3">
+      <c r="I44" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -2085,14 +1950,11 @@
       <c r="H45">
         <v>99.17</v>
       </c>
-      <c r="I45">
-        <v>65.209999999999994</v>
-      </c>
-      <c r="J45" s="3">
+      <c r="I45" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2117,14 +1979,11 @@
       <c r="H46">
         <v>22.68</v>
       </c>
-      <c r="I46">
-        <v>99.14</v>
-      </c>
-      <c r="J46" s="3">
+      <c r="I46" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2149,14 +2008,11 @@
       <c r="H47">
         <v>60.5</v>
       </c>
-      <c r="I47">
-        <v>11.61</v>
-      </c>
-      <c r="J47" s="3">
+      <c r="I47" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2181,14 +2037,11 @@
       <c r="H48">
         <v>95.17</v>
       </c>
-      <c r="I48">
-        <v>38.19</v>
-      </c>
-      <c r="J48" s="3">
+      <c r="I48" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2213,14 +2066,11 @@
       <c r="H49">
         <v>28.12</v>
       </c>
-      <c r="I49">
-        <v>58.88</v>
-      </c>
-      <c r="J49" s="3">
+      <c r="I49" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2245,14 +2095,11 @@
       <c r="H50">
         <v>95.76</v>
       </c>
-      <c r="I50">
-        <v>70.709999999999994</v>
-      </c>
-      <c r="J50" s="3">
+      <c r="I50" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2277,14 +2124,11 @@
       <c r="H51">
         <v>19.09</v>
       </c>
-      <c r="I51">
-        <v>95.51</v>
-      </c>
-      <c r="J51" s="3">
+      <c r="I51" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2309,14 +2153,11 @@
       <c r="H52">
         <v>68.83</v>
       </c>
-      <c r="I52">
-        <v>99.46</v>
-      </c>
-      <c r="J52" s="3">
+      <c r="I52" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2341,14 +2182,11 @@
       <c r="H53">
         <v>99.65</v>
       </c>
-      <c r="I53">
-        <v>86.42</v>
-      </c>
-      <c r="J53" s="3">
+      <c r="I53" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -2373,14 +2211,11 @@
       <c r="H54">
         <v>21.75</v>
       </c>
-      <c r="I54">
-        <v>13.41</v>
-      </c>
-      <c r="J54" s="3">
+      <c r="I54" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -2405,14 +2240,11 @@
       <c r="H55">
         <v>36.770000000000003</v>
       </c>
-      <c r="I55">
-        <v>70.180000000000007</v>
-      </c>
-      <c r="J55" s="3">
+      <c r="I55" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -2437,14 +2269,11 @@
       <c r="H56">
         <v>33</v>
       </c>
-      <c r="I56">
-        <v>93.63</v>
-      </c>
-      <c r="J56" s="3">
+      <c r="I56" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2469,14 +2298,11 @@
       <c r="H57">
         <v>56.16</v>
       </c>
-      <c r="I57">
-        <v>85.99</v>
-      </c>
-      <c r="J57" s="3">
+      <c r="I57" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -2501,14 +2327,11 @@
       <c r="H58">
         <v>31.74</v>
       </c>
-      <c r="I58">
-        <v>65.41</v>
-      </c>
-      <c r="J58" s="3">
+      <c r="I58" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -2533,14 +2356,11 @@
       <c r="H59">
         <v>53.24</v>
       </c>
-      <c r="I59">
-        <v>45.53</v>
-      </c>
-      <c r="J59" s="3">
+      <c r="I59" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2565,14 +2385,11 @@
       <c r="H60">
         <v>84.7</v>
       </c>
-      <c r="I60">
-        <v>38.06</v>
-      </c>
-      <c r="J60" s="3">
+      <c r="I60" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -2597,14 +2414,11 @@
       <c r="H61">
         <v>17.309999999999999</v>
       </c>
-      <c r="I61">
-        <v>61.47</v>
-      </c>
-      <c r="J61" s="3">
+      <c r="I61" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2629,14 +2443,11 @@
       <c r="H62">
         <v>72.36</v>
       </c>
-      <c r="I62">
-        <v>33.950000000000003</v>
-      </c>
-      <c r="J62" s="3">
+      <c r="I62" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -2661,14 +2472,11 @@
       <c r="H63">
         <v>77.290000000000006</v>
       </c>
-      <c r="I63">
-        <v>50.44</v>
-      </c>
-      <c r="J63" s="3">
+      <c r="I63" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2693,14 +2501,11 @@
       <c r="H64">
         <v>82.36</v>
       </c>
-      <c r="I64">
-        <v>46.99</v>
-      </c>
-      <c r="J64" s="3">
+      <c r="I64" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2725,14 +2530,11 @@
       <c r="H65">
         <v>80.91</v>
       </c>
-      <c r="I65">
-        <v>81.92</v>
-      </c>
-      <c r="J65" s="3">
+      <c r="I65" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -2757,14 +2559,11 @@
       <c r="H66">
         <v>62.27</v>
       </c>
-      <c r="I66">
-        <v>67.319999999999993</v>
-      </c>
-      <c r="J66" s="3">
+      <c r="I66" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2789,14 +2588,11 @@
       <c r="H67">
         <v>75.98</v>
       </c>
-      <c r="I67">
-        <v>16.18</v>
-      </c>
-      <c r="J67" s="3">
+      <c r="I67" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2821,14 +2617,11 @@
       <c r="H68">
         <v>55.98</v>
       </c>
-      <c r="I68">
-        <v>49.38</v>
-      </c>
-      <c r="J68" s="3">
+      <c r="I68" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2853,10 +2646,7 @@
       <c r="H69">
         <v>86.88</v>
       </c>
-      <c r="I69">
-        <v>59.26</v>
-      </c>
-      <c r="J69" s="3">
+      <c r="I69" s="3">
         <v>51</v>
       </c>
     </row>

</xml_diff>